<commit_message>
test con ID [48], riportare in colonna “Messaggio di errore”, l’errore visualizzato a video dall’utente, e in colonna “Gestione errore”, le modalità di gestione dell’errore ritornato dal Gateway
modificato test id 162
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/asl2savonese/onesys-amb/2.6.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/asl2savonese/onesys-amb/2.6.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACCREDITAMENTO_FSE_ONESYS\GATEWAY\A1#111ELCO0000000\asl2savonese\onesys-amb\2.6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90610857-008F-474D-950A-BA91879B6833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F1CD39-30AB-4959-8A2D-A24372EFBBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="949">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4586,12 +4586,6 @@
 </t>
   </si>
   <si>
-    <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
-    <t>In automatico prima di inviare a fse o al repository viene tentata nuova validazione</t>
-  </si>
-  <si>
     <t>Non è gestito il Quesito Clinico Attraverso codici loinc</t>
   </si>
   <si>
@@ -4757,9 +4751,6 @@
     <t>906cf1dfef58a3a3</t>
   </si>
   <si>
-    <t>"[ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text']"</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.0c5327d87e19191ac838ef4f8b4cf706afed218e46165d64cc6cc34d4d8869e9.ba77b2fb49^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -4872,6 +4863,19 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.10.4.4.7102.eff5785005717996e796b439401a77b75087a9a055a73f6e54612707146230f7.44a9879603^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Timeout di connessione verso il gateway nazionale. Si desidera continuare?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"[ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text']"
+</t>
+  </si>
+  <si>
+    <t>Il medico qualora conosca il quesito clinico (che dovrebbe arrivare dalla prescrizione) potrà correggere l'errore e proseguire</t>
+  </si>
+  <si>
+    <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2. Per rieffettuare la validazione occorrerà rifirmare il referto</t>
   </si>
 </sst>
 </file>
@@ -7782,10 +7786,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I154" sqref="I154"/>
+      <selection pane="bottomRight" activeCell="P154" sqref="P154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7828,7 +7832,7 @@
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="40" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="D2" s="39"/>
       <c r="F2" s="12"/>
@@ -7853,7 +7857,7 @@
       </c>
       <c r="B3" s="42"/>
       <c r="C3" s="47" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="D3" s="39"/>
       <c r="F3" s="12"/>
@@ -7876,7 +7880,7 @@
       <c r="A4" s="43"/>
       <c r="B4" s="44"/>
       <c r="C4" s="47" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="D4" s="39"/>
       <c r="E4" s="4"/>
@@ -7900,7 +7904,7 @@
       <c r="A5" s="45"/>
       <c r="B5" s="46"/>
       <c r="C5" s="47" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="D5" s="39"/>
       <c r="F5" s="12"/>
@@ -9044,13 +9048,13 @@
         <v>45251</v>
       </c>
       <c r="G39" s="24" t="s">
+        <v>855</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>856</v>
+      </c>
+      <c r="I39" s="24" t="s">
         <v>857</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>858</v>
-      </c>
-      <c r="I39" s="24" t="s">
-        <v>859</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>139</v>
@@ -9336,13 +9340,13 @@
         <v>45251</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>139</v>
@@ -9616,7 +9620,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="120.75" thickBot="1">
+    <row r="55" spans="1:20" ht="210.75" thickBot="1">
       <c r="A55" s="20">
         <v>48</v>
       </c>
@@ -9636,7 +9640,7 @@
         <v>45251</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="H55" s="24"/>
       <c r="I55" s="24"/>
@@ -9651,13 +9655,13 @@
         <v>139</v>
       </c>
       <c r="N55" s="33" t="s">
-        <v>852</v>
+        <v>945</v>
       </c>
       <c r="O55" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="P55" s="25" t="s">
-        <v>853</v>
+      <c r="P55" s="33" t="s">
+        <v>948</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -13026,13 +13030,13 @@
         <v>45252</v>
       </c>
       <c r="G154" s="34" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="H154" s="34" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="I154" s="34" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="J154" s="25" t="s">
         <v>139</v>
@@ -13074,7 +13078,7 @@
         <v>848</v>
       </c>
       <c r="K155" s="33" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="L155" s="25"/>
       <c r="M155" s="25"/>
@@ -13112,7 +13116,7 @@
         <v>848</v>
       </c>
       <c r="K156" s="33" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -13150,7 +13154,7 @@
         <v>848</v>
       </c>
       <c r="K157" s="33" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -13184,13 +13188,13 @@
         <v>45251</v>
       </c>
       <c r="G158" s="24" t="s">
+        <v>864</v>
+      </c>
+      <c r="H158" s="24" t="s">
         <v>866</v>
       </c>
-      <c r="H158" s="24" t="s">
-        <v>868</v>
-      </c>
       <c r="I158" s="24" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="J158" s="25" t="s">
         <v>139</v>
@@ -13203,13 +13207,13 @@
         <v>139</v>
       </c>
       <c r="N158" s="33" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="O158" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P158" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q158" s="25"/>
       <c r="R158" s="26"/>
@@ -13238,13 +13242,13 @@
         <v>45251</v>
       </c>
       <c r="G159" s="24" t="s">
+        <v>867</v>
+      </c>
+      <c r="H159" s="24" t="s">
         <v>869</v>
       </c>
-      <c r="H159" s="24" t="s">
-        <v>871</v>
-      </c>
       <c r="I159" s="24" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="J159" s="25" t="s">
         <v>139</v>
@@ -13257,13 +13261,13 @@
         <v>139</v>
       </c>
       <c r="N159" s="25" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="O159" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P159" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q159" s="25"/>
       <c r="R159" s="26"/>
@@ -13292,13 +13296,13 @@
         <v>45251</v>
       </c>
       <c r="G160" s="24" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="H160" s="24" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="I160" s="24" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="J160" s="25" t="s">
         <v>139</v>
@@ -13311,13 +13315,13 @@
         <v>139</v>
       </c>
       <c r="N160" s="25" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="O160" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P160" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q160" s="25"/>
       <c r="R160" s="26"/>
@@ -13346,13 +13350,13 @@
         <v>45251</v>
       </c>
       <c r="G161" s="24" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="H161" s="24" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="I161" s="24" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="J161" s="25" t="s">
         <v>139</v>
@@ -13365,13 +13369,13 @@
         <v>139</v>
       </c>
       <c r="N161" s="25" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="O161" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P161" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q161" s="25"/>
       <c r="R161" s="26"/>
@@ -13400,13 +13404,13 @@
         <v>45251</v>
       </c>
       <c r="G162" s="24" t="s">
+        <v>880</v>
+      </c>
+      <c r="H162" s="24" t="s">
         <v>882</v>
       </c>
-      <c r="H162" s="24" t="s">
-        <v>884</v>
-      </c>
       <c r="I162" s="24" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="J162" s="25" t="s">
         <v>139</v>
@@ -13419,13 +13423,13 @@
         <v>139</v>
       </c>
       <c r="N162" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="O162" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P162" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q162" s="25"/>
       <c r="R162" s="26"/>
@@ -13454,13 +13458,13 @@
         <v>45251</v>
       </c>
       <c r="G163" s="24" t="s">
+        <v>884</v>
+      </c>
+      <c r="H163" s="24" t="s">
         <v>886</v>
       </c>
-      <c r="H163" s="24" t="s">
-        <v>888</v>
-      </c>
       <c r="I163" s="24" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="J163" s="25" t="s">
         <v>139</v>
@@ -13473,13 +13477,13 @@
         <v>139</v>
       </c>
       <c r="N163" s="25" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="O163" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P163" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26"/>
@@ -13508,13 +13512,13 @@
         <v>45251</v>
       </c>
       <c r="G164" s="24" t="s">
+        <v>888</v>
+      </c>
+      <c r="H164" s="24" t="s">
         <v>890</v>
       </c>
-      <c r="H164" s="24" t="s">
-        <v>892</v>
-      </c>
       <c r="I164" s="24" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="J164" s="25" t="s">
         <v>139</v>
@@ -13527,13 +13531,13 @@
         <v>139</v>
       </c>
       <c r="N164" s="25" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="O164" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P164" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q164" s="25"/>
       <c r="R164" s="26"/>
@@ -13562,13 +13566,13 @@
         <v>45251</v>
       </c>
       <c r="G165" s="34" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="H165" s="34" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="I165" s="34" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="J165" s="25" t="s">
         <v>139</v>
@@ -13581,13 +13585,13 @@
         <v>139</v>
       </c>
       <c r="N165" s="33" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="O165" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P165" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q165" s="25"/>
       <c r="R165" s="26"/>
@@ -13616,13 +13620,13 @@
         <v>45251</v>
       </c>
       <c r="G166" s="34" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="H166" s="34" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="I166" s="34" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="J166" s="25" t="s">
         <v>139</v>
@@ -13635,13 +13639,13 @@
         <v>139</v>
       </c>
       <c r="N166" s="33" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="O166" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P166" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q166" s="25"/>
       <c r="R166" s="26"/>
@@ -13670,13 +13674,13 @@
         <v>45251</v>
       </c>
       <c r="G167" s="34" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H167" s="34" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="I167" s="34" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="J167" s="25" t="s">
         <v>139</v>
@@ -13689,13 +13693,13 @@
         <v>139</v>
       </c>
       <c r="N167" s="33" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="O167" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P167" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
@@ -13724,13 +13728,13 @@
         <v>45251</v>
       </c>
       <c r="G168" s="34" t="s">
+        <v>904</v>
+      </c>
+      <c r="H168" s="34" t="s">
         <v>906</v>
       </c>
-      <c r="H168" s="34" t="s">
-        <v>908</v>
-      </c>
       <c r="I168" s="34" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="J168" s="25" t="s">
         <v>139</v>
@@ -13743,13 +13747,13 @@
         <v>139</v>
       </c>
       <c r="N168" s="33" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="O168" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P168" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26"/>
@@ -13778,13 +13782,13 @@
         <v>45251</v>
       </c>
       <c r="G169" s="34" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="H169" s="34" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="I169" s="34" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="J169" s="25" t="s">
         <v>139</v>
@@ -13797,13 +13801,13 @@
         <v>139</v>
       </c>
       <c r="N169" s="33" t="s">
-        <v>909</v>
+        <v>946</v>
       </c>
       <c r="O169" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P169" s="33" t="s">
-        <v>856</v>
+        <v>947</v>
       </c>
       <c r="Q169" s="25"/>
       <c r="R169" s="26"/>
@@ -13832,13 +13836,13 @@
         <v>45251</v>
       </c>
       <c r="G170" s="34" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="H170" s="34" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="I170" s="34" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="J170" s="25" t="s">
         <v>139</v>
@@ -13851,13 +13855,13 @@
         <v>139</v>
       </c>
       <c r="N170" s="33" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="O170" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P170" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q170" s="25"/>
       <c r="R170" s="26"/>
@@ -13886,13 +13890,13 @@
         <v>45251</v>
       </c>
       <c r="G171" s="34" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="H171" s="34" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="I171" s="34" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="J171" s="25" t="s">
         <v>139</v>
@@ -13905,13 +13909,13 @@
         <v>139</v>
       </c>
       <c r="N171" s="33" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="O171" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P171" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q171" s="25"/>
       <c r="R171" s="26"/>
@@ -13940,13 +13944,13 @@
         <v>45251</v>
       </c>
       <c r="G172" s="34" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="H172" s="34" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="I172" s="34" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="J172" s="25" t="s">
         <v>139</v>
@@ -13959,13 +13963,13 @@
         <v>139</v>
       </c>
       <c r="N172" s="33" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="O172" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P172" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q172" s="25"/>
       <c r="R172" s="26"/>
@@ -13994,13 +13998,13 @@
         <v>45251</v>
       </c>
       <c r="G173" s="24" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="H173" s="34" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="I173" s="34" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="J173" s="25" t="s">
         <v>139</v>
@@ -14013,13 +14017,13 @@
         <v>139</v>
       </c>
       <c r="N173" s="33" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="O173" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P173" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q173" s="25"/>
       <c r="R173" s="26"/>
@@ -14048,13 +14052,13 @@
         <v>45251</v>
       </c>
       <c r="G174" s="34" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="H174" s="34" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="I174" s="34" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="J174" s="25" t="s">
         <v>139</v>
@@ -14067,13 +14071,13 @@
         <v>139</v>
       </c>
       <c r="N174" s="33" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="O174" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P174" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q174" s="25"/>
       <c r="R174" s="26"/>
@@ -14102,13 +14106,13 @@
         <v>45251</v>
       </c>
       <c r="G175" s="34" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="H175" s="34" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="I175" s="34" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="J175" s="25" t="s">
         <v>139</v>
@@ -14121,13 +14125,13 @@
         <v>139</v>
       </c>
       <c r="N175" s="33" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="O175" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P175" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q175" s="25"/>
       <c r="R175" s="26"/>
@@ -14156,13 +14160,13 @@
         <v>45251</v>
       </c>
       <c r="G176" s="34" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="H176" s="34" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="I176" s="34" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="J176" s="25" t="s">
         <v>139</v>
@@ -14175,13 +14179,13 @@
         <v>139</v>
       </c>
       <c r="N176" s="33" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="O176" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P176" s="33" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="Q176" s="25"/>
       <c r="R176" s="26"/>
@@ -21146,13 +21150,13 @@
         <v>45251</v>
       </c>
       <c r="G381" s="24" t="s">
+        <v>861</v>
+      </c>
+      <c r="H381" s="24" t="s">
+        <v>862</v>
+      </c>
+      <c r="I381" s="24" t="s">
         <v>863</v>
-      </c>
-      <c r="H381" s="24" t="s">
-        <v>864</v>
-      </c>
-      <c r="I381" s="24" t="s">
-        <v>865</v>
       </c>
       <c r="J381" s="25" t="s">
         <v>139</v>

</xml_diff>